<commit_message>
autofits and bolds the headers
did the changes on main lol
</commit_message>
<xml_diff>
--- a/IS303p3.xlsx
+++ b/IS303p3.xlsx
@@ -22,13 +22,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -51,8 +54,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,19 +429,24 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="7" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Class Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Student Info</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>
@@ -3161,24 +3170,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Last Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>First Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>ID Number</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>
@@ -4052,24 +4067,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Last Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>First Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>ID Number</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>
@@ -4843,24 +4864,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Last Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>First Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>ID Number</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>
@@ -5614,24 +5641,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Last Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>First Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>ID Number</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>
@@ -6365,24 +6398,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Last Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>First Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>ID Number</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Grade</t>
         </is>

</xml_diff>